<commit_message>
Conversão clínica → barbearia + remoção de autenticação + deploy guides
</commit_message>
<xml_diff>
--- a/services/agendamentos.xlsx
+++ b/services/agendamentos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>07/11/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Samuk derik</t>
+          <t>Samuel Bispo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12345678909</t>
+          <t>55290347801</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>5511917281651@c.us</t>
+          <t>5511915742431@c.us</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -511,388 +511,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-10-27 20:48:27</t>
+          <t>2025-11-07 21:36:36</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>27/10/2025_08:00_5511917281651@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>27/10/2025</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>08:30</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Kkfjaj shsje</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>22/08/2001</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5511917281651@c.us</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2025-10-27 20:50:02</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>27/10/2025_08:30_5511917281651@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Samuel Bispo</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>28/10/1999</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>5511917281651@c.us</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2025-10-28 15:23:06</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>28/10/2025_08:00_5511917281651@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>samuquinha Bispo</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>05/06/2005</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>5511917281651@c.us</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2025-10-28 15:24:28</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>28/10/2025_09:00_5511917281651@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>samuel bispo</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>17/06/2005</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>5511917281651@c.us</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2025-10-28 15:33:28</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>28/10/2025_10:00_5511917281651@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Aroldo bispo</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>17/12/2005</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>5511915742431@c.us</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2025-10-28 16:41:41</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>28/10/2025_11:00_5511915742431@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>29/10/2025</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Muquinha bispo</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>04/05/2000</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>5511915742431@c.us</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2025-10-29 00:09:39</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>29/10/2025_08:00_5511915742431@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>07/12/2025</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>leandro silva</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>12345678909</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>5511915742431@c.us</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Confirmado</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2025-10-29 01:33:38</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>07/12/2025_08:00_5511915742431@c.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>31/10/2025</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>André Reis</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12/05/1985</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>33481116845</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>5511982888582@c.us</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Pendente Pagamento</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2025-10-31 01:57:55</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>31/10/2025_17:00_5511982888582@c.us</t>
+          <t>07/11/2025_08:00_5511915742431@c.us</t>
         </is>
       </c>
     </row>

</xml_diff>